<commit_message>
Final models and updated for 1 and 2
</commit_message>
<xml_diff>
--- a/barb_progress.xlsx
+++ b/barb_progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="0" windowWidth="21160" windowHeight="14740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1720" yWindow="0" windowWidth="21160" windowHeight="14740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assign 1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="66">
   <si>
     <t>SVM</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>MLAssignment2_7</t>
+  </si>
+  <si>
+    <t>8th Attempt</t>
+  </si>
+  <si>
+    <t>MLAssignment2_8</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -304,6 +310,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -424,7 +434,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -505,6 +515,8 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
@@ -557,6 +569,8 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -890,7 +904,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2385,13 +2399,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC36"/>
+  <dimension ref="A1:AC41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2991,6 +3005,82 @@
       </c>
       <c r="F36" s="2">
         <v>0.04</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="4" customFormat="1"/>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="2">
+        <v>57319450.729999997</v>
+      </c>
+      <c r="D38" s="2">
+        <v>81629775.769999996</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="G38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="2">
+        <v>58311575.32</v>
+      </c>
+      <c r="D40" s="2">
+        <v>80243320.760000005</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="2">
+        <v>74602382.700000003</v>
+      </c>
+      <c r="D41" s="2">
+        <v>87764855.879999995</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>